<commit_message>
task 1 finishedgit add .
</commit_message>
<xml_diff>
--- a/Test_Sets/Project_Sets/src/main/resources/projects60.xlsx
+++ b/Test_Sets/Project_Sets/src/main/resources/projects60.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="120">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,361 +26,352 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Don Vito Corleone</t>
-  </si>
-  <si>
-    <t>the Mafia and the Dagon mythos</t>
+    <t>Freddie Mercury</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Robinson Crusoe</t>
+  </si>
+  <si>
+    <t>English literature and the Dagon mythos</t>
   </si>
   <si>
     <t>DS</t>
   </si>
   <si>
-    <t xml:space="preserve"> The Godfather and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a crime family in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>John Lennon</t>
-  </si>
-  <si>
-    <t>The Beatles and the Cthulu-Dagon mythos</t>
+    <t xml:space="preserve"> Desert Islands and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>making home-made clothes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Norma Desmond</t>
+  </si>
+  <si>
+    <t>Sunset Boulevard and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>clinging to past dreams in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Darth Maul</t>
+  </si>
+  <si>
+    <t>Star Wars and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Dark Side and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting the Dark Side in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Timothy McGee</t>
+  </si>
+  <si>
+    <t>NCIS and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>solving mysteries in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Lt. George Colthurst St Barleigh</t>
+  </si>
+  <si>
+    <t>the English class system and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>providing comic relief in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stephen Hawking</t>
+  </si>
+  <si>
+    <t>Physics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modern science and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Cosmos and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Quentin Tarantino</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu-Dagon mythos</t>
   </si>
   <si>
     <t>CS+DS</t>
   </si>
   <si>
-    <t xml:space="preserve"> Pop music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>writing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Keith Moon</t>
-  </si>
-  <si>
-    <t>Rock music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>playing drums in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> raising cain in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sauron</t>
-  </si>
-  <si>
-    <t>Lord of the Rings and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Middle Earth and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mordor and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Iggy Pop</t>
-  </si>
-  <si>
-    <t>Music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jazz and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Blues music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>O.J. Simpson</t>
-  </si>
-  <si>
-    <t>American football and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing golf in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making threatening phone calls in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Bruce Banner</t>
-  </si>
-  <si>
-    <t>Marvel Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>flying into a rage in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bursting out of shirts in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>P. T. Barnum</t>
-  </si>
-  <si>
-    <t>the Circus and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Showmanship and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting circus attractions in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mr. Bean</t>
-  </si>
-  <si>
-    <t>British comedy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British humour and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>causing mayhem in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Uriah Heap</t>
-  </si>
-  <si>
-    <t>David Copperfield and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dickensian fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Dian Fossey</t>
-  </si>
-  <si>
-    <t>Rwanda and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gorillas and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zoology and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Neville Chamberlain</t>
-  </si>
-  <si>
-    <t>World War II and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>appeasing belligerent dictators in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Warren Buffett</t>
-  </si>
-  <si>
-    <t>Big business and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Modern finance and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>running a business empire in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Wyatt Earp</t>
-  </si>
-  <si>
-    <t>The Old West and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Westerns and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>arresting criminals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Andrew Lloyd Webber</t>
-  </si>
-  <si>
-    <t>Musicals and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Musical Theatre and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>making insipid musicals in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Melania Trump</t>
+    <t xml:space="preserve"> Indie Movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making violent movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Che Guevara</t>
+  </si>
+  <si>
+    <t>Cuban politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Cuban revolution and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cuba and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Morrissey</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Alexander Fleming</t>
+  </si>
+  <si>
+    <t>Science and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Biology and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>studying science in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Otto von Bismarck</t>
+  </si>
+  <si>
+    <t>German history and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> German politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>wielding political power in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Grace Kelly</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Monacco and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Dean Winchester</t>
+  </si>
+  <si>
+    <t>Horror and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Supernatural and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Demonology and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Frida Kahlo</t>
+  </si>
+  <si>
+    <t>Mexican art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>painting colorful pictures in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>David Letterman</t>
+  </si>
+  <si>
+    <t>Late-night TV and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chat Shows and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CBS and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Harvey Weinstein</t>
+  </si>
+  <si>
+    <t>chasing after women in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> seducing women in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Johannes Gutenberg</t>
+  </si>
+  <si>
+    <t>Printing and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>pioneering new technologies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Hillary Clinton</t>
   </si>
   <si>
     <t>American politics and the Cthulu mythos</t>
   </si>
   <si>
-    <t>posing for photographs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Newt Gingrich</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Woody Guthrie</t>
-  </si>
-  <si>
-    <t>Folk music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>campaigning for environmental causes in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> campaigning for social causes in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Angela Merkel</t>
-  </si>
-  <si>
-    <t>Politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> European politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Germany and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Jar Jar Binks</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>providing comic relief in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Gore Vidal</t>
-  </si>
-  <si>
-    <t>American literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Modern literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing modern fiction in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Garry Trudeau</t>
-  </si>
-  <si>
-    <t>Doonesbury and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Political Cartoons and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>drawing political cartoons in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Shirley Temple</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu-Dagon mythos</t>
+    <t xml:space="preserve"> the Left and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Democrats and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>King Lear</t>
+  </si>
+  <si>
+    <t>Shakespeare and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>going senile in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Buzz Lightyear</t>
+  </si>
+  <si>
+    <t>Pixar and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Toy Story and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>falling gracefully in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Harriet Tubman</t>
+  </si>
+  <si>
+    <t>American history and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>fighting for civil rights in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Howard Stern</t>
+  </si>
+  <si>
+    <t>Talk radio and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>shocking radio listeners in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hosting radio shows in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Carl Lewis</t>
+  </si>
+  <si>
+    <t>Athletics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Olympics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>winning gold medals in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Erasmus</t>
+  </si>
+  <si>
+    <t>Humanism and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting humanism in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jim Morrison</t>
+  </si>
+  <si>
+    <t>Rock music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Galileo Galilei</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Astronomy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting Heliocentrism in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jay Gatsby</t>
+  </si>
+  <si>
+    <t>The Great Gatsby and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>throwing lavish parties in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>John Belushi</t>
+  </si>
+  <si>
+    <t>Comedy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Orson Welles</t>
   </si>
   <si>
     <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
   </si>
   <si>
-    <t>starring in Hollywood movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Offred</t>
-  </si>
-  <si>
-    <t>Science Fiction and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Handmaid's Tale and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>performing household chores in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Kobe Bryant</t>
-  </si>
-  <si>
-    <t>Basketball and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing basketball in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making dunk shots in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Robbie Williams</t>
-  </si>
-  <si>
-    <t>Pop music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Take That and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jerry Seinfeld</t>
-  </si>
-  <si>
-    <t>The Seinfeld Chronicles and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>doing stand-up in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Alan Greenspan</t>
-  </si>
-  <si>
-    <t>Economics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>talking up the economy in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Nigella Lawson</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Noël Coward</t>
-  </si>
-  <si>
-    <t>British theatre and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing plays in Cthulhu-worshipping societies</t>
+    <t xml:space="preserve"> Serious Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>directing Hollywood movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
   </si>
 </sst>
 </file>
@@ -456,7 +447,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>1.505783055364567E-5</v>
+        <v>1.5712109037655364E-5</v>
       </c>
     </row>
     <row r="3">
@@ -470,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>2.1651536583204518E-5</v>
+        <v>2.2882974782502155E-5</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +475,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>3.086452805560744E-5</v>
+        <v>3.301861938558835E-5</v>
       </c>
     </row>
     <row r="5">
@@ -498,7 +489,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>4.3618945181192063E-5</v>
+        <v>4.720345305784465E-5</v>
       </c>
     </row>
     <row r="6">
@@ -512,7 +503,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>6.111323578402071E-5</v>
+        <v>6.685856663314933E-5</v>
       </c>
     </row>
     <row r="7">
@@ -526,7 +517,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>8.488676861496594E-5</v>
+        <v>9.382288586223318E-5</v>
       </c>
     </row>
     <row r="8">
@@ -537,10 +528,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>1.1689322142142652E-4</v>
+        <v>1.3044545353947022E-4</v>
       </c>
     </row>
     <row r="9">
@@ -548,13 +539,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>1.595817624250387E-4</v>
+        <v>1.7968736598590222E-4</v>
       </c>
     </row>
     <row r="10">
@@ -562,228 +553,228 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>2.1598410522086274E-4</v>
+        <v>2.4523055113574927E-4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>2.898043709736888E-4</v>
+        <v>3.3158894511433506E-4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.855073630913083E-4</v>
+        <v>4.4421574738256683E-4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>5.083994008726104E-4</v>
+        <v>5.895983997792394E-4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>6.646943545436847E-4</v>
+        <v>7.753308807374694E-4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
         <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>8.615560933513725E-4</v>
+        <v>0.001010151023383744</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001107107352715952</v>
+        <v>0.001303929094273841</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0014103942251250208</v>
+        <v>0.0016675930842951102</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0017812952787859193</v>
+        <v>0.0021129763580244017</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0022303649055994993</v>
+        <v>0.002652574764543515</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
-        <v>32</v>
-      </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>0.002768602073801108</v>
+        <v>0.0032992032661826737</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003407138344583718</v>
+        <v>0.004065546738784504</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004156842869608986</v>
+        <v>0.00496360585532948</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0050278470850103375</v>
+        <v>0.006004046735196597</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D24" t="n">
-        <v>0.006028997807761845</v>
+        <v>0.007195471982361319</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>0.007167254142553786</v>
+        <v>0.008543640303901062</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
@@ -792,12 +783,12 @@
         <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>0.008447050610743002</v>
+        <v>0.010050671362960006</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
@@ -806,133 +797,133 @@
         <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>0.009869655688586887</v>
+        <v>0.011714280995660964</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D28" t="n">
-        <v>0.011432560872336073</v>
+        <v>0.013527098443184227</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D29" t="n">
-        <v>0.013128939812225127</v>
+        <v>0.015476120857530695</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="D30" t="n">
-        <v>0.014947219331531203</v>
+        <v>0.017542360183192884</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="n">
-        <v>0.016870803711083293</v>
+        <v>0.019700732972561807</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D32" t="n">
-        <v>0.018877990070226114</v>
+        <v>0.021920234466040966</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>0.020942105831001756</v>
+        <v>0.02416442447891065</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D34" t="n">
-        <v>0.023031889205752942</v>
+        <v>0.026392234869326625</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D35" t="n">
-        <v>0.025112120796158655</v>
+        <v>0.028559087662930138</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>0.02714449943490027</v>
+        <v>0.03061829073868061</v>
       </c>
     </row>
     <row r="37">
@@ -943,10 +934,10 @@
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D37" t="n">
-        <v>0.029088739313355316</v>
+        <v>0.032522656101615754</v>
       </c>
     </row>
     <row r="38">
@@ -957,10 +948,10 @@
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D38" t="n">
-        <v>0.030903849400578998</v>
+        <v>0.034226266096593155</v>
       </c>
     </row>
     <row r="39">
@@ -971,10 +962,10 @@
         <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03254954146350572</v>
+        <v>0.035686297332261474</v>
       </c>
     </row>
     <row r="40">
@@ -988,7 +979,7 @@
         <v>11</v>
       </c>
       <c r="D40" t="n">
-        <v>0.03398770093550979</v>
+        <v>0.036864802230996724</v>
       </c>
     </row>
     <row r="41">
@@ -1002,7 +993,7 @@
         <v>11</v>
       </c>
       <c r="D41" t="n">
-        <v>0.03518384661026934</v>
+        <v>0.03773034521835793</v>
       </c>
     </row>
     <row r="42">
@@ -1016,7 +1007,7 @@
         <v>11</v>
       </c>
       <c r="D42" t="n">
-        <v>0.036108501568554774</v>
+        <v>0.0382593952557892</v>
       </c>
     </row>
     <row r="43">
@@ -1027,10 +1018,10 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03673839942888419</v>
+        <v>0.03843738866572659</v>
       </c>
     </row>
     <row r="44">
@@ -1041,10 +1032,10 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0370574570707446</v>
+        <v>0.03825939525578885</v>
       </c>
     </row>
     <row r="45">
@@ -1055,10 +1046,10 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0370574570707446</v>
+        <v>0.03773034521835811</v>
       </c>
     </row>
     <row r="46">
@@ -1069,10 +1060,10 @@
         <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D46" t="n">
-        <v>0.036738399428884315</v>
+        <v>0.03686480223099682</v>
       </c>
     </row>
     <row r="47">
@@ -1083,94 +1074,94 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D47" t="n">
-        <v>0.036108501568554566</v>
+        <v>0.03568629733226136</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" t="s">
         <v>69</v>
       </c>
-      <c r="B48" t="s">
-        <v>70</v>
-      </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D48" t="n">
-        <v>0.035183846610269284</v>
+        <v>0.0342262660965931</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
         <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03398770093550993</v>
+        <v>0.03252265610161595</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
         <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D50" t="n">
-        <v>0.03254954146350572</v>
+        <v>0.030618290738680443</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
         <v>73</v>
       </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D51" t="n">
-        <v>0.030903849400578998</v>
+        <v>0.02855908766293025</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>0.029088739313355205</v>
+        <v>0.026392234869326403</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D53" t="n">
-        <v>0.02714449943490016</v>
+        <v>0.024164424478910818</v>
       </c>
     </row>
     <row r="54">
@@ -1181,10 +1172,10 @@
         <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>0.025112120796158877</v>
+        <v>0.021920234466040966</v>
       </c>
     </row>
     <row r="55">
@@ -1195,10 +1186,10 @@
         <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D55" t="n">
-        <v>0.023031889205752942</v>
+        <v>0.01970073297256164</v>
       </c>
     </row>
     <row r="56">
@@ -1209,10 +1200,10 @@
         <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D56" t="n">
-        <v>0.020942105831001756</v>
+        <v>0.01754236018319294</v>
       </c>
     </row>
     <row r="57">
@@ -1223,10 +1214,10 @@
         <v>82</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D57" t="n">
-        <v>0.018877990070226225</v>
+        <v>0.01547612085753075</v>
       </c>
     </row>
     <row r="58">
@@ -1237,10 +1228,10 @@
         <v>83</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D58" t="n">
-        <v>0.016870803711083127</v>
+        <v>0.013527098443184116</v>
       </c>
     </row>
     <row r="59">
@@ -1251,10 +1242,10 @@
         <v>85</v>
       </c>
       <c r="C59" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D59" t="n">
-        <v>0.014947219331531258</v>
+        <v>0.011714280995660964</v>
       </c>
     </row>
     <row r="60">
@@ -1265,10 +1256,10 @@
         <v>86</v>
       </c>
       <c r="C60" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D60" t="n">
-        <v>0.013128939812225127</v>
+        <v>0.010050671362960117</v>
       </c>
     </row>
     <row r="61">
@@ -1279,10 +1270,10 @@
         <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D61" t="n">
-        <v>0.011432560872336073</v>
+        <v>0.008543640303900951</v>
       </c>
     </row>
     <row r="62">
@@ -1293,10 +1284,10 @@
         <v>89</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D62" t="n">
-        <v>0.009869655688586942</v>
+        <v>0.007195471982361333</v>
       </c>
     </row>
     <row r="63">
@@ -1307,234 +1298,234 @@
         <v>90</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>0.008447050610742905</v>
+        <v>0.006004046735196614</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B64" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0071672541425537376</v>
+        <v>0.004963605855329449</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B65" t="s">
         <v>93</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.006028997807761935</v>
+        <v>0.004065546738784509</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
         <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0050278470850103375</v>
+        <v>0.0032992032661826754</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>0.004156842869608986</v>
+        <v>0.002652574764543508</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B68" t="s">
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D68" t="n">
-        <v>0.003407138344583697</v>
+        <v>0.002112976358024406</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B69" t="s">
         <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0027686020738011026</v>
+        <v>0.0016675930842951162</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D70" t="n">
-        <v>0.0022303649055995254</v>
+        <v>0.0013039290942738306</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B71" t="s">
         <v>101</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0017812952787859193</v>
+        <v>0.0010101510233837515</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0014103942251250208</v>
+        <v>7.753308807374672E-4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C73" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0011071073527159432</v>
+        <v>5.895983997792342E-4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
         <v>105</v>
       </c>
       <c r="C74" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D74" t="n">
-        <v>8.615560933513768E-4</v>
+        <v>4.4421574738256965E-4</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>6.646943545436891E-4</v>
+        <v>3.315889451143343E-4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C76" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>5.083994008726104E-4</v>
+        <v>2.452305511357472E-4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
         <v>11</v>
       </c>
       <c r="D77" t="n">
-        <v>3.855073630913083E-4</v>
+        <v>1.7968736598590222E-4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
         <v>11</v>
       </c>
       <c r="D78" t="n">
-        <v>2.898043709736888E-4</v>
+        <v>1.3044545353947104E-4</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D79" t="n">
-        <v>2.1598410522086155E-4</v>
+        <v>9.382288586223236E-5</v>
       </c>
     </row>
     <row r="80">
@@ -1542,13 +1533,13 @@
         <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D80" t="n">
-        <v>1.5958176242503988E-4</v>
+        <v>6.68585666331496E-5</v>
       </c>
     </row>
     <row r="81">
@@ -1556,97 +1547,55 @@
         <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D81" t="n">
-        <v>1.1689322142142652E-4</v>
+        <v>4.7203453057844376E-5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D82" t="n">
-        <v>8.488676861496594E-5</v>
+        <v>3.301861938558857E-5</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D83" t="n">
-        <v>6.111323578402071E-5</v>
+        <v>2.288297478250206E-5</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C84" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="D84" t="n">
-        <v>4.361894518119189E-5</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" t="s">
-        <v>120</v>
-      </c>
-      <c r="C85" t="s">
-        <v>16</v>
-      </c>
-      <c r="D85" t="n">
-        <v>3.08645280556074E-5</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>119</v>
-      </c>
-      <c r="B86" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86" t="s">
-        <v>16</v>
-      </c>
-      <c r="D86" t="n">
-        <v>2.1651536583204735E-5</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>119</v>
-      </c>
-      <c r="B87" t="s">
-        <v>122</v>
-      </c>
-      <c r="C87" t="s">
-        <v>16</v>
-      </c>
-      <c r="D87" t="n">
-        <v>1.505783055364567E-5</v>
+        <v>1.5712109037655242E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>